<commit_message>
mcd finalisé, script mcd finalisé, script des table par generatedata
</commit_message>
<xml_diff>
--- a/Work_Plan.xlsx
+++ b/Work_Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Nom du projet :</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Achevé</t>
   </si>
   <si>
-    <t>En cours</t>
-  </si>
-  <si>
     <t>Non commencé</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>achevé</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>en cours</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color rgb="FF008A3E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,7 +253,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF008A3E"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,11 +490,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -853,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -871,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -880,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -889,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -900,7 +903,7 @@
     </row>
     <row r="6" spans="1:44" ht="18.75">
       <c r="A6" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="28">
         <v>44334</v>
@@ -909,7 +912,7 @@
     </row>
     <row r="7" spans="1:44" ht="18.75">
       <c r="A7" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="28">
         <v>44414</v>
@@ -925,6 +928,9 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
+      <c r="AC9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:44" ht="30" customHeight="1">
       <c r="A10" s="16" t="s">
@@ -960,25 +966,63 @@
       <c r="K10" s="10">
         <v>44337</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="10"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="10"/>
+      <c r="L10" s="10">
+        <v>44342</v>
+      </c>
+      <c r="M10" s="10">
+        <v>44343</v>
+      </c>
+      <c r="N10" s="10">
+        <v>44344</v>
+      </c>
+      <c r="O10" s="10">
+        <v>44345</v>
+      </c>
+      <c r="P10" s="10">
+        <v>44346</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>44347</v>
+      </c>
+      <c r="R10" s="10">
+        <v>44348</v>
+      </c>
+      <c r="S10" s="10">
+        <v>44349</v>
+      </c>
+      <c r="T10" s="10">
+        <v>44350</v>
+      </c>
+      <c r="U10" s="10">
+        <v>44351</v>
+      </c>
+      <c r="V10" s="10">
+        <v>44352</v>
+      </c>
+      <c r="W10" s="10">
+        <v>44353</v>
+      </c>
+      <c r="X10" s="10">
+        <v>44354</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>44355</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>44356</v>
+      </c>
+      <c r="AA10" s="10">
+        <v>44357</v>
+      </c>
+      <c r="AB10" s="10">
+        <v>44358</v>
+      </c>
+      <c r="AC10" s="10">
+        <v>44359</v>
+      </c>
+      <c r="AD10" s="10">
+        <v>44360</v>
+      </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
@@ -1044,10 +1088,10 @@
     </row>
     <row r="12" spans="1:44" ht="48.75" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="9">
         <v>44333</v>
@@ -1103,10 +1147,10 @@
     </row>
     <row r="13" spans="1:44" ht="52.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9">
         <v>44334</v>
@@ -1213,7 +1257,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9">
         <v>44334</v>
@@ -1269,10 +1313,10 @@
     </row>
     <row r="16" spans="1:44" ht="64.5" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="9">
         <v>44334</v>
@@ -1284,8 +1328,8 @@
         <f>D16-C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="43" t="s">
-        <v>35</v>
+      <c r="F16" s="42" t="s">
+        <v>34</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1426,7 +1470,7 @@
     </row>
     <row r="19" spans="1:44" ht="22.15" customHeight="1">
       <c r="A19" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1474,10 +1518,10 @@
     </row>
     <row r="20" spans="1:44" ht="51" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="9">
         <v>44335</v>
@@ -1490,15 +1534,15 @@
         <v>0</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="1"/>
       <c r="I20" s="38"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1533,10 +1577,10 @@
     </row>
     <row r="21" spans="1:44" ht="58.5" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9">
         <v>44336</v>
@@ -1548,21 +1592,23 @@
         <f>D21-C21</f>
         <v>0</v>
       </c>
-      <c r="F21" s="42" t="s">
-        <v>13</v>
+      <c r="F21" s="41" t="s">
+        <v>12</v>
       </c>
       <c r="G21" s="13"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="38"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1592,10 +1638,10 @@
     </row>
     <row r="22" spans="1:44" ht="98.25" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1603,8 +1649,8 @@
         <f t="shared" ref="E22:E25" si="0">D22-C22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="39" t="s">
-        <v>14</v>
+      <c r="F22" s="43" t="s">
+        <v>36</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="1"/>
@@ -1618,7 +1664,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="S22" s="38"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -1645,12 +1691,12 @@
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
     </row>
-    <row r="23" spans="1:44" ht="79.5" customHeight="1">
+    <row r="23" spans="1:44" ht="70.5" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1659,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="1"/>
@@ -1702,10 +1748,10 @@
     </row>
     <row r="24" spans="1:44" ht="59.25" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1714,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="1"/>
@@ -1757,10 +1803,10 @@
     </row>
     <row r="25" spans="1:44" ht="141.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1769,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="1"/>
@@ -1812,7 +1858,7 @@
     </row>
     <row r="26" spans="1:44" ht="22.15" customHeight="1">
       <c r="A26" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1860,10 +1906,10 @@
     </row>
     <row r="27" spans="1:44" ht="63" customHeight="1">
       <c r="A27" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1872,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="1"/>
@@ -1915,16 +1961,16 @@
     </row>
     <row r="28" spans="1:44" ht="54" customHeight="1">
       <c r="A28" s="35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="3"/>
       <c r="F28" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="1"/>
@@ -1967,10 +2013,10 @@
     </row>
     <row r="29" spans="1:44" ht="69" customHeight="1">
       <c r="A29" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1979,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="1"/>
@@ -2022,10 +2068,10 @@
     </row>
     <row r="30" spans="1:44" ht="60.75" customHeight="1">
       <c r="A30" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2034,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="1"/>

</xml_diff>

<commit_message>
mcd finalisé, script des tables, script base wazaaimmo, script tester la base, création des utilisateurs, privileges, rôle
</commit_message>
<xml_diff>
--- a/Work_Plan.xlsx
+++ b/Work_Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Nom du projet :</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>en cours</t>
+  </si>
+  <si>
+    <t>Concepteur du site</t>
+  </si>
+  <si>
+    <t>Amirat Youcef</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -254,6 +260,14 @@
       <b/>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +403,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -451,12 +465,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -496,6 +506,26 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -854,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AR37"/>
+  <dimension ref="A1:AR37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -869,59 +899,67 @@
     <col min="7" max="44" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:44" ht="18.75">
+    <row r="1" spans="1:44" ht="25.5" customHeight="1">
+      <c r="A1" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="26.25" customHeight="1">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:44" ht="18.75">
+    <row r="3" spans="1:44" ht="47.25">
       <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:44" ht="18.75">
+    <row r="4" spans="1:44" ht="48">
       <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="45" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:44" ht="18.75">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:44" ht="18.75">
+    <row r="6" spans="1:44" ht="24" customHeight="1">
       <c r="A6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="46">
         <v>44334</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:44" ht="18.75">
+    <row r="7" spans="1:44" ht="28.5" customHeight="1">
       <c r="A7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="47">
         <v>44414</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:44" ht="18.75">
       <c r="A8" s="24"/>
-      <c r="B8" s="29"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:44">
@@ -1090,7 +1128,7 @@
       <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="9">
@@ -1106,7 +1144,7 @@
       <c r="F12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="38"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1149,7 +1187,7 @@
       <c r="A13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9">
@@ -1166,7 +1204,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="38"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1253,10 +1291,10 @@
       <c r="AR14" s="11"/>
     </row>
     <row r="15" spans="1:44" ht="51.75" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="9">
@@ -1273,9 +1311,9 @@
         <v>12</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1315,26 +1353,26 @@
       <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="9">
         <v>44334</v>
       </c>
       <c r="D16" s="9">
-        <v>44334</v>
+        <v>44335</v>
       </c>
       <c r="E16" s="3">
         <f>D16-C16</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="40" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="35"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1469,7 +1507,7 @@
       <c r="AR18" s="1"/>
     </row>
     <row r="19" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4"/>
@@ -1520,29 +1558,29 @@
       <c r="A20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="9">
         <v>44335</v>
       </c>
       <c r="D20" s="9">
-        <v>44335</v>
+        <v>44339</v>
       </c>
       <c r="E20" s="3">
         <f>D20-C20</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="39" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1579,20 +1617,20 @@
       <c r="A21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="9">
         <v>44336</v>
       </c>
       <c r="D21" s="9">
-        <v>44336</v>
+        <v>44348</v>
       </c>
       <c r="E21" s="3">
         <f>D21-C21</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="13"/>
@@ -1603,12 +1641,12 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="38"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="38"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1640,17 +1678,21 @@
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+      <c r="C22" s="9">
+        <v>44349</v>
+      </c>
+      <c r="D22" s="9">
+        <v>44357</v>
+      </c>
       <c r="E22" s="3">
         <f t="shared" ref="E22:E25" si="0">D22-C22</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>36</v>
+        <v>8</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>12</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="1"/>
@@ -1664,15 +1706,15 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="38"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="36"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
+      <c r="X22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36"/>
+      <c r="AA22" s="36"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -1695,17 +1737,19 @@
       <c r="A23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9">
+        <v>44358</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="39" t="s">
-        <v>13</v>
+        <v>-44358</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>36</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="1"/>
@@ -1728,7 +1772,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
+      <c r="AB23" s="36"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
@@ -1750,7 +1794,7 @@
       <c r="A24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="9"/>
@@ -1759,7 +1803,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="13"/>
@@ -1805,7 +1849,7 @@
       <c r="A25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="9"/>
@@ -1814,7 +1858,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G25" s="13"/>
@@ -1857,14 +1901,14 @@
       <c r="AR25" s="1"/>
     </row>
     <row r="26" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="40"/>
+      <c r="F26" s="38"/>
       <c r="G26" s="12"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
@@ -1905,10 +1949,10 @@
       <c r="AR26" s="11"/>
     </row>
     <row r="27" spans="1:44" ht="63" customHeight="1">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="9"/>
@@ -1917,7 +1961,7 @@
         <f>D27-C27</f>
         <v>0</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G27" s="13"/>
@@ -1960,16 +2004,16 @@
       <c r="AR27" s="1"/>
     </row>
     <row r="28" spans="1:44" ht="54" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="13"/>
@@ -2012,10 +2056,10 @@
       <c r="AR28" s="1"/>
     </row>
     <row r="29" spans="1:44" ht="69" customHeight="1">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="9"/>
@@ -2024,7 +2068,7 @@
         <f>B33-A33</f>
         <v>0</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="13"/>
@@ -2067,10 +2111,10 @@
       <c r="AR29" s="1"/>
     </row>
     <row r="30" spans="1:44" ht="60.75" customHeight="1">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="9"/>
@@ -2079,7 +2123,7 @@
         <f>B33-A33</f>
         <v>0</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="37" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="13"/>
@@ -2122,7 +2166,7 @@
       <c r="AR30" s="1"/>
     </row>
     <row r="31" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A31" s="35"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="3"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2168,7 +2212,7 @@
       <c r="AR31" s="1"/>
     </row>
     <row r="32" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A32" s="35"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="3"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2258,12 +2302,12 @@
       <c r="AP33" s="1"/>
     </row>
     <row r="34" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="34"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2304,11 +2348,11 @@
       <c r="AR34" s="2"/>
     </row>
     <row r="35" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A35" s="32"/>
-      <c r="B35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="34"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2349,11 +2393,11 @@
       <c r="AR35" s="2"/>
     </row>
     <row r="36" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A36" s="32"/>
-      <c r="B36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="34"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>

</xml_diff>

<commit_message>
partie base de données et mcd
</commit_message>
<xml_diff>
--- a/Work_Plan.xlsx
+++ b/Work_Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Nom du projet :</t>
   </si>
@@ -129,13 +129,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Concepteur du site</t>
+  </si>
+  <si>
+    <t>Amirat Youcef</t>
+  </si>
+  <si>
+    <t>construction de la maquette</t>
+  </si>
+  <si>
     <t>en cours</t>
-  </si>
-  <si>
-    <t>Concepteur du site</t>
-  </si>
-  <si>
-    <t>Amirat Youcef</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,22 +261,36 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="9"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +318,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +426,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -459,9 +482,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -503,9 +523,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -525,7 +542,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -884,85 +906,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR37"/>
+  <dimension ref="A1:AY35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="1" max="1" width="43.625" customWidth="1"/>
     <col min="2" max="2" width="15.25" customWidth="1"/>
     <col min="3" max="5" width="10.75" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="44" width="4.5" customWidth="1"/>
+    <col min="7" max="45" width="4.5" customWidth="1"/>
+    <col min="46" max="46" width="3.75" customWidth="1"/>
+    <col min="47" max="47" width="3.875" customWidth="1"/>
+    <col min="48" max="49" width="3.5" customWidth="1"/>
+    <col min="50" max="50" width="3.875" customWidth="1"/>
+    <col min="51" max="51" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="25.5" customHeight="1">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:51" ht="25.5" customHeight="1">
+      <c r="A1" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" ht="26.25" customHeight="1">
-      <c r="A2" s="24" t="s">
+    </row>
+    <row r="2" spans="1:51" ht="26.25" customHeight="1">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:44" ht="47.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:51" ht="47.25">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:44" ht="48">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:51" ht="48">
+      <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="43" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:44" ht="18.75">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+    <row r="5" spans="1:51" ht="18.75">
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:44" ht="24" customHeight="1">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:51" ht="24" customHeight="1">
+      <c r="A6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="44">
         <v>44334</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:44" ht="28.5" customHeight="1">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:51" ht="28.5" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="45">
         <v>44414</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:44" ht="18.75">
-      <c r="A8" s="24"/>
-      <c r="B8" s="27"/>
+    <row r="8" spans="1:51" ht="18.75">
+      <c r="A8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:51">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -970,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="30" customHeight="1">
+    <row r="10" spans="1:51" ht="30" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>3</v>
       </c>
@@ -1061,22 +1088,51 @@
       <c r="AD10" s="10">
         <v>44360</v>
       </c>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AH10" s="10"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" s="10"/>
-      <c r="AO10" s="10"/>
+      <c r="AE10" s="10">
+        <v>44361</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>44362</v>
+      </c>
+      <c r="AG10" s="10">
+        <v>44363</v>
+      </c>
+      <c r="AH10" s="10">
+        <v>44364</v>
+      </c>
+      <c r="AI10" s="48">
+        <v>44365</v>
+      </c>
+      <c r="AJ10" s="10">
+        <v>44366</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>44367</v>
+      </c>
+      <c r="AL10" s="10">
+        <v>44368</v>
+      </c>
+      <c r="AM10" s="10">
+        <v>44369</v>
+      </c>
+      <c r="AN10" s="10">
+        <v>44370</v>
+      </c>
+      <c r="AO10" s="10">
+        <v>44371</v>
+      </c>
       <c r="AP10" s="10"/>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="10"/>
-    </row>
-    <row r="11" spans="1:44" ht="23.25" customHeight="1">
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
+      <c r="AX10" s="10"/>
+      <c r="AY10" s="10"/>
+    </row>
+    <row r="11" spans="1:51" ht="23.25" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
@@ -1123,12 +1179,19 @@
       <c r="AP11" s="11"/>
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
-    </row>
-    <row r="12" spans="1:44" ht="48.75" customHeight="1">
+      <c r="AS11" s="11"/>
+      <c r="AT11" s="11"/>
+      <c r="AU11" s="11"/>
+      <c r="AV11" s="11"/>
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="11"/>
+      <c r="AY11" s="11"/>
+    </row>
+    <row r="12" spans="1:51" ht="48.75" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="9">
@@ -1144,7 +1207,7 @@
       <c r="F12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="36"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1182,12 +1245,19 @@
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
       <c r="AR12" s="1"/>
-    </row>
-    <row r="13" spans="1:44" ht="52.5" customHeight="1">
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1"/>
+    </row>
+    <row r="13" spans="1:51" ht="52.5" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9">
@@ -1204,7 +1274,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="36"/>
+      <c r="H13" s="35"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1241,8 +1311,15 @@
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
       <c r="AR13" s="1"/>
-    </row>
-    <row r="14" spans="1:44" ht="22.15" customHeight="1">
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="1"/>
+    </row>
+    <row r="14" spans="1:51" ht="22.15" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
@@ -1289,12 +1366,19 @@
       <c r="AP14" s="11"/>
       <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
-    </row>
-    <row r="15" spans="1:44" ht="51.75" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="AS14" s="11"/>
+      <c r="AT14" s="11"/>
+      <c r="AU14" s="11"/>
+      <c r="AV14" s="11"/>
+      <c r="AW14" s="11"/>
+      <c r="AX14" s="11"/>
+      <c r="AY14" s="11"/>
+    </row>
+    <row r="15" spans="1:51" ht="51.75" customHeight="1">
+      <c r="A15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="9">
@@ -1311,9 +1395,9 @@
         <v>12</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1348,12 +1432,19 @@
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
-    </row>
-    <row r="16" spans="1:44" ht="64.5" customHeight="1">
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="1"/>
+      <c r="AY15" s="1"/>
+    </row>
+    <row r="16" spans="1:51" ht="64.5" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="9">
@@ -1366,13 +1457,13 @@
         <f>D16-C16</f>
         <v>1</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="39" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="34"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1407,8 +1498,15 @@
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
-    </row>
-    <row r="17" spans="1:44">
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+    </row>
+    <row r="17" spans="1:51">
       <c r="A17" s="18"/>
       <c r="B17" s="3"/>
       <c r="C17" s="9"/>
@@ -1456,8 +1554,15 @@
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
-    </row>
-    <row r="18" spans="1:44" ht="22.15" customHeight="1">
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+    </row>
+    <row r="18" spans="1:51" ht="22.15" customHeight="1">
       <c r="A18" s="20"/>
       <c r="B18" s="3"/>
       <c r="C18" s="9"/>
@@ -1505,9 +1610,16 @@
       <c r="AP18" s="1"/>
       <c r="AQ18" s="1"/>
       <c r="AR18" s="1"/>
-    </row>
-    <row r="19" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A19" s="28" t="s">
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="1"/>
+    </row>
+    <row r="19" spans="1:51" ht="22.15" customHeight="1">
+      <c r="A19" s="27" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="4"/>
@@ -1553,12 +1665,19 @@
       <c r="AP19" s="11"/>
       <c r="AQ19" s="11"/>
       <c r="AR19" s="11"/>
-    </row>
-    <row r="20" spans="1:44" ht="51" customHeight="1">
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="11"/>
+      <c r="AV19" s="11"/>
+      <c r="AW19" s="11"/>
+      <c r="AX19" s="11"/>
+      <c r="AY19" s="11"/>
+    </row>
+    <row r="20" spans="1:51" ht="51" customHeight="1">
       <c r="A20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="9">
@@ -1571,16 +1690,16 @@
         <f>D20-C20</f>
         <v>4</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="38" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1612,12 +1731,19 @@
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
       <c r="AR20" s="1"/>
-    </row>
-    <row r="21" spans="1:44" ht="58.5" customHeight="1">
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1"/>
+      <c r="AU20" s="1"/>
+      <c r="AV20" s="1"/>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="1"/>
+    </row>
+    <row r="21" spans="1:51" ht="58.5" customHeight="1">
       <c r="A21" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="9">
@@ -1630,7 +1756,7 @@
         <f>D21-C21</f>
         <v>12</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="38" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="13"/>
@@ -1641,12 +1767,12 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1673,12 +1799,19 @@
       <c r="AP21" s="1"/>
       <c r="AQ21" s="1"/>
       <c r="AR21" s="1"/>
-    </row>
-    <row r="22" spans="1:44" ht="98.25" customHeight="1">
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1"/>
+    </row>
+    <row r="22" spans="1:51" ht="98.25" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="9">
@@ -1691,7 +1824,7 @@
         <f t="shared" ref="E22:E25" si="0">D22-C22</f>
         <v>8</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="40" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="13"/>
@@ -1706,15 +1839,15 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="36"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="35"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
@@ -1732,24 +1865,33 @@
       <c r="AP22" s="1"/>
       <c r="AQ22" s="1"/>
       <c r="AR22" s="1"/>
-    </row>
-    <row r="23" spans="1:44" ht="70.5" customHeight="1">
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1"/>
+    </row>
+    <row r="23" spans="1:51" ht="70.5" customHeight="1">
       <c r="A23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="9">
         <v>44358</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9">
+        <v>44361</v>
+      </c>
       <c r="E23" s="3">
         <f t="shared" si="0"/>
-        <v>-44358</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>12</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="1"/>
@@ -1772,7 +1914,7 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
-      <c r="AB23" s="36"/>
+      <c r="AB23" s="35"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
@@ -1789,22 +1931,33 @@
       <c r="AP23" s="1"/>
       <c r="AQ23" s="1"/>
       <c r="AR23" s="1"/>
-    </row>
-    <row r="24" spans="1:44" ht="59.25" customHeight="1">
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="1"/>
+    </row>
+    <row r="24" spans="1:51" ht="59.25" customHeight="1">
       <c r="A24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
+      <c r="C24" s="9">
+        <v>44358</v>
+      </c>
+      <c r="D24" s="9">
+        <v>44361</v>
+      </c>
       <c r="E24" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>12</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="1"/>
@@ -1830,7 +1983,7 @@
       <c r="AB24" s="1"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
-      <c r="AE24" s="1"/>
+      <c r="AE24" s="35"/>
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
@@ -1844,22 +1997,33 @@
       <c r="AP24" s="1"/>
       <c r="AQ24" s="1"/>
       <c r="AR24" s="1"/>
-    </row>
-    <row r="25" spans="1:44" ht="141.75" customHeight="1">
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="1"/>
+    </row>
+    <row r="25" spans="1:51" ht="141.75" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="9">
+        <v>44361</v>
+      </c>
+      <c r="D25" s="9">
+        <v>44364</v>
+      </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>12</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="1"/>
@@ -1885,10 +2049,10 @@
       <c r="AB25" s="1"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
-      <c r="AF25" s="1"/>
-      <c r="AG25" s="1"/>
-      <c r="AH25" s="1"/>
+      <c r="AE25" s="35"/>
+      <c r="AF25" s="35"/>
+      <c r="AG25" s="35"/>
+      <c r="AH25" s="35"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -1899,16 +2063,23 @@
       <c r="AP25" s="1"/>
       <c r="AQ25" s="1"/>
       <c r="AR25" s="1"/>
-    </row>
-    <row r="26" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A26" s="28" t="s">
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="1"/>
+    </row>
+    <row r="26" spans="1:51" ht="22.15" customHeight="1">
+      <c r="A26" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="38"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="12"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
@@ -1947,22 +2118,33 @@
       <c r="AP26" s="11"/>
       <c r="AQ26" s="11"/>
       <c r="AR26" s="11"/>
-    </row>
-    <row r="27" spans="1:44" ht="63" customHeight="1">
-      <c r="A27" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="33" t="s">
+      <c r="AS26" s="11"/>
+      <c r="AT26" s="11"/>
+      <c r="AU26" s="11"/>
+      <c r="AV26" s="11"/>
+      <c r="AW26" s="11"/>
+      <c r="AX26" s="11"/>
+      <c r="AY26" s="11"/>
+    </row>
+    <row r="27" spans="1:51" ht="63" customHeight="1">
+      <c r="A27" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
+      <c r="C27" s="9">
+        <v>44364</v>
+      </c>
+      <c r="D27" s="9">
+        <v>44365</v>
+      </c>
       <c r="E27" s="3">
         <f>D27-C27</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>39</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="1"/>
@@ -1991,7 +2173,7 @@
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
+      <c r="AH27" s="50"/>
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -2002,18 +2184,25 @@
       <c r="AP27" s="1"/>
       <c r="AQ27" s="1"/>
       <c r="AR27" s="1"/>
-    </row>
-    <row r="28" spans="1:44" ht="54" customHeight="1">
-      <c r="A28" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="33" t="s">
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="1"/>
+    </row>
+    <row r="28" spans="1:51" ht="63" customHeight="1">
+      <c r="A28" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="36" t="s">
         <v>13</v>
       </c>
       <c r="G28" s="13"/>
@@ -2054,21 +2243,25 @@
       <c r="AP28" s="1"/>
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
-    </row>
-    <row r="29" spans="1:44" ht="69" customHeight="1">
-      <c r="A29" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="33" t="s">
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1"/>
+    </row>
+    <row r="29" spans="1:51" ht="54" customHeight="1">
+      <c r="A29" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="3">
-        <f>B33-A33</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="37" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="36" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="13"/>
@@ -2109,21 +2302,28 @@
       <c r="AP29" s="1"/>
       <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
-    </row>
-    <row r="30" spans="1:44" ht="60.75" customHeight="1">
-      <c r="A30" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="33" t="s">
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="1"/>
+    </row>
+    <row r="30" spans="1:51" ht="69" customHeight="1">
+      <c r="A30" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="3">
-        <f>B33-A33</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="37" t="s">
+      <c r="E30" s="3" t="e">
+        <f>#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F30" s="36" t="s">
         <v>13</v>
       </c>
       <c r="G30" s="13"/>
@@ -2164,14 +2364,30 @@
       <c r="AP30" s="1"/>
       <c r="AQ30" s="1"/>
       <c r="AR30" s="1"/>
-    </row>
-    <row r="31" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="3"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1"/>
+      <c r="AU30" s="1"/>
+      <c r="AV30" s="1"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+      <c r="AY30" s="1"/>
+    </row>
+    <row r="31" spans="1:51" ht="60.75" customHeight="1">
+      <c r="A31" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="23"/>
+      <c r="E31" s="3" t="e">
+        <f>#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="G31" s="13"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2210,104 +2426,111 @@
       <c r="AP31" s="1"/>
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
-    </row>
-    <row r="32" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A32" s="33"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AE32" s="1"/>
-      <c r="AF32" s="1"/>
-      <c r="AG32" s="1"/>
-      <c r="AH32" s="1"/>
-      <c r="AI32" s="1"/>
-      <c r="AJ32" s="1"/>
-      <c r="AK32" s="1"/>
-      <c r="AL32" s="1"/>
-      <c r="AM32" s="1"/>
-      <c r="AN32" s="1"/>
-      <c r="AO32" s="1"/>
-      <c r="AP32" s="1"/>
-      <c r="AQ32" s="1"/>
-      <c r="AR32" s="1"/>
+      <c r="AS31" s="1"/>
+      <c r="AT31" s="1"/>
+      <c r="AU31" s="1"/>
+      <c r="AV31" s="1"/>
+      <c r="AW31" s="1"/>
+      <c r="AX31" s="1"/>
+      <c r="AY31" s="1"/>
+    </row>
+    <row r="32" spans="1:51" ht="22.15" customHeight="1">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+      <c r="AP32" s="2"/>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="2"/>
     </row>
     <row r="33" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-      <c r="AG33" s="1"/>
-      <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
-      <c r="AK33" s="1"/>
-      <c r="AL33" s="1"/>
-      <c r="AM33" s="1"/>
-      <c r="AN33" s="1"/>
-      <c r="AO33" s="1"/>
-      <c r="AP33" s="1"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="2"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="2"/>
     </row>
     <row r="34" spans="1:44" ht="22.15" customHeight="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="32"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2347,97 +2570,7 @@
       <c r="AQ34" s="2"/>
       <c r="AR34" s="2"/>
     </row>
-    <row r="35" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2"/>
-      <c r="AG35" s="2"/>
-      <c r="AH35" s="2"/>
-      <c r="AI35" s="2"/>
-      <c r="AJ35" s="2"/>
-      <c r="AK35" s="2"/>
-      <c r="AL35" s="2"/>
-      <c r="AM35" s="2"/>
-      <c r="AN35" s="2"/>
-      <c r="AO35" s="2"/>
-      <c r="AP35" s="2"/>
-      <c r="AQ35" s="2"/>
-      <c r="AR35" s="2"/>
-    </row>
-    <row r="36" spans="1:44" ht="22.15" customHeight="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
-      <c r="AE36" s="2"/>
-      <c r="AF36" s="2"/>
-      <c r="AG36" s="2"/>
-      <c r="AH36" s="2"/>
-      <c r="AI36" s="2"/>
-      <c r="AJ36" s="2"/>
-      <c r="AK36" s="2"/>
-      <c r="AL36" s="2"/>
-      <c r="AM36" s="2"/>
-      <c r="AN36" s="2"/>
-      <c r="AO36" s="2"/>
-      <c r="AP36" s="2"/>
-      <c r="AQ36" s="2"/>
-      <c r="AR36" s="2"/>
-    </row>
-    <row r="37" spans="1:44" ht="28.9" customHeight="1"/>
+    <row r="35" spans="1:44" ht="28.9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>